<commit_message>
Added Table 1 and text about Clinton Administration
</commit_message>
<xml_diff>
--- a/LiteratureReview/docs/POLS6330_2020_Spring_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/LiteratureReview/docs/POLS6330_2020_Spring_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Figure 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Total</t>
   </si>
@@ -71,6 +72,37 @@
   </si>
   <si>
     <t>* indicates preliminary calculation</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Fiscal Year</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Federal Obligations to Universities for 
+Research and Development</t>
+  </si>
+  <si>
+    <t>(Nominal Millions of U.S. Dollars)</t>
+  </si>
+  <si>
+    <t>National Science Foundation, National Center for Science and Engineering Statistics. (2020).</t>
+  </si>
+  <si>
+    <t>May 7, 2020 from http://www.nsf.gov/statistics/fedfunds/</t>
+  </si>
+  <si>
+    <t>Survey of Federal Funds for Research and Development, Fiscal Years 2018-19. Retrieved</t>
+  </si>
+  <si>
+    <t>Data source:</t>
+  </si>
+  <si>
+    <t>Table created by author.</t>
   </si>
 </sst>
 </file>
@@ -135,12 +167,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -149,7 +192,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -200,6 +243,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -220,6 +293,518 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Federal Obligations to Universities</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for Research and Development</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Figure 1'!$A$35:$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019*</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Figure 1'!$B$35:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>16890.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20065.099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21620</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23005.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24947</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25687.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24669.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25547.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26026.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31557.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31192.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27680.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27509.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25772</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27429.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27414.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28199.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28963.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31534.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33359.199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF07-4D4D-885B-B944DECFA80C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="744411736"/>
+        <c:axId val="744415344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="744411736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fiscal Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="744415344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="744415344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions of Nominal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> US Dollars</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="744411736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -719,7 +1304,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1244,518 +1829,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Federal Obligations to Universities</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> for Research and Development</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet3!$A$35:$A$54</c:f>
-              <c:strCache>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2019*</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet3!$B$35:$B$54</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0_);\("$"#,##0\)</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>16890.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20065.099999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21620</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23005.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24947</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25687.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24669.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25547.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>26026.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>31557.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>31192.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>27680.3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>27509.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25772</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>27429.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27414.7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>28199.3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28963.200000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31534.1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>33359.199999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BF07-4D4D-885B-B944DECFA80C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="744411736"/>
-        <c:axId val="744415344"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="744411736"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Fiscal Year</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="744415344"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="744415344"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Millions of Nominal</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> US Dollars</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="744411736"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3390,6 +3463,47 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F7D4F1-F364-4657-9D16-9F8E7A94596F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -3426,7 +3540,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3447,47 +3561,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D659FB0-32AA-45AE-9E5C-A428E08AC8E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>14286</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F7D4F1-F364-4657-9D16-9F8E7A94596F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3805,6 +3878,924 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+    </row>
+    <row r="3" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1967</v>
+      </c>
+      <c r="B6" s="20">
+        <v>1454.3</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1980</v>
+      </c>
+      <c r="E6" s="20">
+        <v>4263.3999999999996</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="20">
+        <v>16890.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1968</v>
+      </c>
+      <c r="B7" s="20">
+        <v>1487.4</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1981</v>
+      </c>
+      <c r="E7" s="20">
+        <v>4465.8</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2001</v>
+      </c>
+      <c r="H7" s="20">
+        <v>20065.099999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>1969</v>
+      </c>
+      <c r="B8" s="20">
+        <v>1529.2</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1982</v>
+      </c>
+      <c r="E8" s="20">
+        <v>4605.5</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2002</v>
+      </c>
+      <c r="H8" s="20">
+        <v>21620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1970</v>
+      </c>
+      <c r="B9" s="20">
+        <v>1475.6</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1983</v>
+      </c>
+      <c r="E9" s="20">
+        <v>4966.3999999999996</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2003</v>
+      </c>
+      <c r="H9" s="20">
+        <v>23005.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>1971</v>
+      </c>
+      <c r="B10" s="20">
+        <v>1644.6</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1984</v>
+      </c>
+      <c r="E10" s="20">
+        <v>5546.9</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2004</v>
+      </c>
+      <c r="H10" s="20">
+        <v>24947</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1972</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1903.5</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1985</v>
+      </c>
+      <c r="E11" s="20">
+        <v>6339.7</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2005</v>
+      </c>
+      <c r="H11" s="20">
+        <v>25687.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1973</v>
+      </c>
+      <c r="B12" s="20">
+        <v>1916.6</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1986</v>
+      </c>
+      <c r="E12" s="20">
+        <v>6558.8</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2006</v>
+      </c>
+      <c r="H12" s="20">
+        <v>24669.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1974</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2214</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1987</v>
+      </c>
+      <c r="E13" s="20">
+        <v>7337.3</v>
+      </c>
+      <c r="G13" s="10">
+        <v>2007</v>
+      </c>
+      <c r="H13" s="20">
+        <v>25547.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1975</v>
+      </c>
+      <c r="B14" s="20">
+        <v>2411.4</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1988</v>
+      </c>
+      <c r="E14" s="20">
+        <v>7827.7</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2008</v>
+      </c>
+      <c r="H14" s="20">
+        <v>26026.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>1976</v>
+      </c>
+      <c r="B15" s="20">
+        <v>2551.8000000000002</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1989</v>
+      </c>
+      <c r="E15" s="20">
+        <v>8672</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2009</v>
+      </c>
+      <c r="H15" s="20">
+        <v>31557.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1977</v>
+      </c>
+      <c r="B16" s="20">
+        <v>2905.5</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1990</v>
+      </c>
+      <c r="E16" s="20">
+        <v>9137.5</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H16" s="20">
+        <v>31192.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1978</v>
+      </c>
+      <c r="B17" s="20">
+        <v>3374.6</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1991</v>
+      </c>
+      <c r="E17" s="20">
+        <v>10168.5</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H17" s="20">
+        <v>27680.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1979</v>
+      </c>
+      <c r="B18" s="20">
+        <v>3888.8</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1992</v>
+      </c>
+      <c r="E18" s="20">
+        <v>10271.200000000001</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H18" s="20">
+        <v>27509.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="10">
+        <v>1993</v>
+      </c>
+      <c r="E19" s="20">
+        <v>11208.4</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2013</v>
+      </c>
+      <c r="H19" s="20">
+        <v>25772</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D20" s="10">
+        <v>1994</v>
+      </c>
+      <c r="E20" s="20">
+        <v>11796.9</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H20" s="20">
+        <v>27429.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="10">
+        <v>1995</v>
+      </c>
+      <c r="E21" s="20">
+        <v>11927.5</v>
+      </c>
+      <c r="G21" s="10">
+        <v>2015</v>
+      </c>
+      <c r="H21" s="20">
+        <v>27414.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="10">
+        <v>1996</v>
+      </c>
+      <c r="E22" s="20">
+        <v>11977.8</v>
+      </c>
+      <c r="G22" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H22" s="20">
+        <v>28199.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="10">
+        <v>1997</v>
+      </c>
+      <c r="E23" s="20">
+        <v>12559</v>
+      </c>
+      <c r="G23" s="10">
+        <v>2017</v>
+      </c>
+      <c r="H23" s="20">
+        <v>28963.200000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="10">
+        <v>1998</v>
+      </c>
+      <c r="E24" s="20">
+        <v>13380.7</v>
+      </c>
+      <c r="G24" s="10">
+        <v>2018</v>
+      </c>
+      <c r="H24" s="20">
+        <v>31534.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="10">
+        <v>1999</v>
+      </c>
+      <c r="E25" s="20">
+        <v>14959.1</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="20">
+        <v>33359.199999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1967</v>
+      </c>
+      <c r="B2" s="19">
+        <v>1454.3</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1968</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1487.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>1969</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1529.2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>1970</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1475.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>1971</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1644.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1972</v>
+      </c>
+      <c r="B7" s="19">
+        <v>1903.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>1973</v>
+      </c>
+      <c r="B8" s="19">
+        <v>1916.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1974</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>1975</v>
+      </c>
+      <c r="B10" s="19">
+        <v>2411.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>1976</v>
+      </c>
+      <c r="B11" s="19">
+        <v>2551.8000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>1977</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2905.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>1978</v>
+      </c>
+      <c r="B13" s="19">
+        <v>3374.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1979</v>
+      </c>
+      <c r="B14" s="19">
+        <v>3888.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>1980</v>
+      </c>
+      <c r="B15" s="19">
+        <v>4263.3999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>1981</v>
+      </c>
+      <c r="B16" s="19">
+        <v>4465.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>1982</v>
+      </c>
+      <c r="B17" s="19">
+        <v>4605.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>1983</v>
+      </c>
+      <c r="B18" s="19">
+        <v>4966.3999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>1984</v>
+      </c>
+      <c r="B19" s="19">
+        <v>5546.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="19">
+        <v>6339.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>1986</v>
+      </c>
+      <c r="B21" s="19">
+        <v>6558.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>1987</v>
+      </c>
+      <c r="B22" s="19">
+        <v>7337.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>1988</v>
+      </c>
+      <c r="B23" s="19">
+        <v>7827.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>1989</v>
+      </c>
+      <c r="B24" s="19">
+        <v>8672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>1990</v>
+      </c>
+      <c r="B25" s="19">
+        <v>9137.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>1991</v>
+      </c>
+      <c r="B26" s="19">
+        <v>10168.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>1992</v>
+      </c>
+      <c r="B27" s="19">
+        <v>10271.200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>1993</v>
+      </c>
+      <c r="B28" s="19">
+        <v>11208.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>1994</v>
+      </c>
+      <c r="B29" s="19">
+        <v>11796.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>1995</v>
+      </c>
+      <c r="B30" s="19">
+        <v>11927.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>1996</v>
+      </c>
+      <c r="B31" s="19">
+        <v>11977.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>1997</v>
+      </c>
+      <c r="B32" s="19">
+        <v>12559</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>1998</v>
+      </c>
+      <c r="B33" s="19">
+        <v>13380.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>1999</v>
+      </c>
+      <c r="B34" s="19">
+        <v>14959.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="19">
+        <v>16890.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>2001</v>
+      </c>
+      <c r="B36" s="19">
+        <v>20065.099999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>2002</v>
+      </c>
+      <c r="B37" s="19">
+        <v>21620</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>2003</v>
+      </c>
+      <c r="B38" s="19">
+        <v>23005.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>2004</v>
+      </c>
+      <c r="B39" s="19">
+        <v>24947</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>2005</v>
+      </c>
+      <c r="B40" s="19">
+        <v>25687.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>2006</v>
+      </c>
+      <c r="B41" s="19">
+        <v>24669.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>2007</v>
+      </c>
+      <c r="B42" s="19">
+        <v>25547.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B43" s="19">
+        <v>26026.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>2009</v>
+      </c>
+      <c r="B44" s="19">
+        <v>31557.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>2010</v>
+      </c>
+      <c r="B45" s="19">
+        <v>31192.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>2011</v>
+      </c>
+      <c r="B46" s="19">
+        <v>27680.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>2012</v>
+      </c>
+      <c r="B47" s="19">
+        <v>27509.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>2013</v>
+      </c>
+      <c r="B48" s="19">
+        <v>25772</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B49" s="19">
+        <v>27429.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>2015</v>
+      </c>
+      <c r="B50" s="19">
+        <v>27414.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>2016</v>
+      </c>
+      <c r="B51" s="19">
+        <v>28199.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>2017</v>
+      </c>
+      <c r="B52" s="19">
+        <v>28963.200000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>2018</v>
+      </c>
+      <c r="B53" s="19">
+        <v>31534.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="19">
+        <v>33359.199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4058,7 +5049,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -4643,465 +5634,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
-        <v>1967</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1454.3</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1968</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1487.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>1969</v>
-      </c>
-      <c r="B4" s="19">
-        <v>1529.2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>1970</v>
-      </c>
-      <c r="B5" s="19">
-        <v>1475.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>1971</v>
-      </c>
-      <c r="B6" s="19">
-        <v>1644.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>1972</v>
-      </c>
-      <c r="B7" s="19">
-        <v>1903.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>1973</v>
-      </c>
-      <c r="B8" s="19">
-        <v>1916.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1974</v>
-      </c>
-      <c r="B9" s="19">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>1975</v>
-      </c>
-      <c r="B10" s="19">
-        <v>2411.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1976</v>
-      </c>
-      <c r="B11" s="19">
-        <v>2551.8000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>1977</v>
-      </c>
-      <c r="B12" s="19">
-        <v>2905.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>1978</v>
-      </c>
-      <c r="B13" s="19">
-        <v>3374.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1979</v>
-      </c>
-      <c r="B14" s="19">
-        <v>3888.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>1980</v>
-      </c>
-      <c r="B15" s="19">
-        <v>4263.3999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>1981</v>
-      </c>
-      <c r="B16" s="19">
-        <v>4465.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>1982</v>
-      </c>
-      <c r="B17" s="19">
-        <v>4605.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1983</v>
-      </c>
-      <c r="B18" s="19">
-        <v>4966.3999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>1984</v>
-      </c>
-      <c r="B19" s="19">
-        <v>5546.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>1985</v>
-      </c>
-      <c r="B20" s="19">
-        <v>6339.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>1986</v>
-      </c>
-      <c r="B21" s="19">
-        <v>6558.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>1987</v>
-      </c>
-      <c r="B22" s="19">
-        <v>7337.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>1988</v>
-      </c>
-      <c r="B23" s="19">
-        <v>7827.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>1989</v>
-      </c>
-      <c r="B24" s="19">
-        <v>8672</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>1990</v>
-      </c>
-      <c r="B25" s="19">
-        <v>9137.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>1991</v>
-      </c>
-      <c r="B26" s="19">
-        <v>10168.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1992</v>
-      </c>
-      <c r="B27" s="19">
-        <v>10271.200000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>1993</v>
-      </c>
-      <c r="B28" s="19">
-        <v>11208.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>1994</v>
-      </c>
-      <c r="B29" s="19">
-        <v>11796.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>1995</v>
-      </c>
-      <c r="B30" s="19">
-        <v>11927.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>1996</v>
-      </c>
-      <c r="B31" s="19">
-        <v>11977.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>1997</v>
-      </c>
-      <c r="B32" s="19">
-        <v>12559</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>1998</v>
-      </c>
-      <c r="B33" s="19">
-        <v>13380.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>1999</v>
-      </c>
-      <c r="B34" s="19">
-        <v>14959.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
-        <v>2000</v>
-      </c>
-      <c r="B35" s="19">
-        <v>16890.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>2001</v>
-      </c>
-      <c r="B36" s="19">
-        <v>20065.099999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
-        <v>2002</v>
-      </c>
-      <c r="B37" s="19">
-        <v>21620</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>2003</v>
-      </c>
-      <c r="B38" s="19">
-        <v>23005.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
-        <v>2004</v>
-      </c>
-      <c r="B39" s="19">
-        <v>24947</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
-        <v>2005</v>
-      </c>
-      <c r="B40" s="19">
-        <v>25687.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
-        <v>2006</v>
-      </c>
-      <c r="B41" s="19">
-        <v>24669.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
-        <v>2007</v>
-      </c>
-      <c r="B42" s="19">
-        <v>25547.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
-        <v>2008</v>
-      </c>
-      <c r="B43" s="19">
-        <v>26026.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
-        <v>2009</v>
-      </c>
-      <c r="B44" s="19">
-        <v>31557.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="10">
-        <v>2010</v>
-      </c>
-      <c r="B45" s="19">
-        <v>31192.3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="10">
-        <v>2011</v>
-      </c>
-      <c r="B46" s="19">
-        <v>27680.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
-        <v>2012</v>
-      </c>
-      <c r="B47" s="19">
-        <v>27509.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
-        <v>2013</v>
-      </c>
-      <c r="B48" s="19">
-        <v>25772</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>2014</v>
-      </c>
-      <c r="B49" s="19">
-        <v>27429.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
-        <v>2015</v>
-      </c>
-      <c r="B50" s="19">
-        <v>27414.7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
-        <v>2016</v>
-      </c>
-      <c r="B51" s="19">
-        <v>28199.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
-        <v>2017</v>
-      </c>
-      <c r="B52" s="19">
-        <v>28963.200000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
-        <v>2018</v>
-      </c>
-      <c r="B53" s="19">
-        <v>31534.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="19">
-        <v>33359.199999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel file with tables and figures
</commit_message>
<xml_diff>
--- a/LiteratureReview/docs/POLS6330_2020_Spring_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
+++ b/LiteratureReview/docs/POLS6330_2020_Spring_Townes_LiteratureReview_Tables-and-Figures_v00.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Figure 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Table 2" sheetId="5" r:id="rId2"/>
+    <sheet name="Figure 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Total</t>
   </si>
@@ -87,9 +88,6 @@
 Research and Development</t>
   </si>
   <si>
-    <t>(Nominal Millions of U.S. Dollars)</t>
-  </si>
-  <si>
     <t>National Science Foundation, National Center for Science and Engineering Statistics. (2020).</t>
   </si>
   <si>
@@ -103,6 +101,157 @@
   </si>
   <si>
     <t>Table created by author.</t>
+  </si>
+  <si>
+    <t>Policy</t>
+  </si>
+  <si>
+    <t>Relevant Provisions</t>
+  </si>
+  <si>
+    <t>Relevant Market Failures</t>
+  </si>
+  <si>
+    <t>Permitted universities, nonprofit firms, and small businesses to take title to inventions derived from federally-funded research as a way incentive these organizations to facilitate the use of the inventions to benefit the public interest.</t>
+  </si>
+  <si>
+    <t>Incomplete markets</t>
+  </si>
+  <si>
+    <t>Mandated that federal laboratories establish an Office of Research and Technology Application (ORTA) to facilitate their active technical cooperation with the private sector.</t>
+  </si>
+  <si>
+    <t>Imperfect information</t>
+  </si>
+  <si>
+    <t>Mandated that federal agencies set aside a specific portion of their extramural research budgets to fund research and development projects within the scope of their agency missions to be performed by small businesses in the private sector.</t>
+  </si>
+  <si>
+    <t>Negative externalities</t>
+  </si>
+  <si>
+    <t>Enabled private sector businesses to enter into joint pre-competitive research and development ventures without violating federal antitrust laws.  Eliminated treble damages in antitrust litigation arising from such ventures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Established the Federal Laboratory Consortium (FLC) for Technology Transfer and enabled government-owned, government-operated federal laboratories (GOGOs) to directly enter into cooperative research and development agreements (CRADAs) with private sector businesses. </t>
+  </si>
+  <si>
+    <t>Information failures</t>
+  </si>
+  <si>
+    <t>Executive Order 12591</t>
+  </si>
+  <si>
+    <t>Executive Order 12618</t>
+  </si>
+  <si>
+    <t>Established Manufacturing Technology Centers and designated the National Institute of Science and Technology (NIST) as the lead agency to administer them.</t>
+  </si>
+  <si>
+    <t>Extended the ability to enter into CRADAs with private sector businesses to all government-owned contractor-operated federal laboratories (GOCOs).</t>
+  </si>
+  <si>
+    <t>Authorizes appropriations to be available for Regional Centers for the Transfer of Manufacturing Technology, State Technology Extension Program, Advanced Technology Program, and Satellite Manufacturing Centers.</t>
+  </si>
+  <si>
+    <t>Directed the Advanced Research Projects Agency (ARPA) to promote dual-use technology via technology reinvestment.</t>
+  </si>
+  <si>
+    <t>Enacted changes to ease the ability of private sector businesses to obtain exclusive license to inventions that result from cooperative research with the federal government.</t>
+  </si>
+  <si>
+    <t>Requires license applicants for federally-owned inventions to commit to achieving practical application of the invention within a reasonable time.</t>
+  </si>
+  <si>
+    <t>Pub.L. 96-517
+Bayh-Dole Act</t>
+  </si>
+  <si>
+    <t>Public goods
+Incomplete markets</t>
+  </si>
+  <si>
+    <t>Pub.L. 96-480
+Stevenson-Wydler 
+Technology Innovation Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 97-219
+Small Business Innovation Development Act</t>
+  </si>
+  <si>
+    <t>Imperfect information
+Imperfect competition
+Negative externalities</t>
+  </si>
+  <si>
+    <t>Pub.L. 98-462
+National Cooperative Research Act</t>
+  </si>
+  <si>
+    <t>Public goods
+Free rider problems
+Imperfect information</t>
+  </si>
+  <si>
+    <t>Pub.L. 99-502
+Federal Technology Transfer Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 102-245
+American Technology 
+Preeminence Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 103-160
+Defense Authorization Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 104-113
+National Technology Transfer and Advancement Act</t>
+  </si>
+  <si>
+    <t>Further specified Pub.L. 99-502 
+for administrative purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sources: </t>
+  </si>
+  <si>
+    <t>Feberallabs. (2013, December 23). Technology Transfer Laws [Video file]. Retrieved from https://youtu.be/k9CEPfku5DI</t>
+  </si>
+  <si>
+    <t>H.R.1989 – American Technology Preeminence Act of 1991. (n.d.). Congress.gov. Retrieved April 23, 2020 from https://www.congress.gov/bill/102nd-congress/house-bill/1989</t>
+  </si>
+  <si>
+    <t>H.R.209 – Technology Transfer Commercialization Act of 2000. (n.d.). Congress.gov. Retrieved April 23, 2020 from https://www.congress.gov/bill/106th-congress/house-bill/209</t>
+  </si>
+  <si>
+    <t>Lee, Y. S. (1997). Technology transfer and economic development: A framework for policy analysis. In Y. S. Lee (Ed.), Technology Transfer and Public Policy (pp. 3-20). Quorum Books.</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Federal Legislation and Executive Action Relevant to University Technology Transfer</t>
+  </si>
+  <si>
+    <t>Pub.L. 106-129
+Technology Transfer 
+Commercialization Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 101-189
+National Competitiveness 
+Technology Transfer Act</t>
+  </si>
+  <si>
+    <t>Pub.L. 100-418
+Ominbus Trade and 
+Competitiveness Act</t>
+  </si>
+  <si>
+    <t>(Millions of Nominal U.S. Dollars)</t>
   </si>
 </sst>
 </file>
@@ -113,7 +262,7 @@
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +307,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +324,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,13 +343,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -258,9 +424,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -272,6 +435,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3893,49 +4080,49 @@
     <col min="8" max="8" width="10.7109375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="22"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" spans="1:8" s="23" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4304,27 +4491,27 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -4335,11 +4522,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="23" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30">
+        <v>1980</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30">
+        <v>1980</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>1982</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>1984</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>1986</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>1987</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>1987</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>1988</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>1989</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30">
+        <v>1991</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>1993</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>1995</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>2000</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+    </row>
+    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+    </row>
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D28">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <mergeCells count="4">
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4794,7 +5376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -5049,13 +5631,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>